<commit_message>
Feat: 학교 url 변경
</commit_message>
<xml_diff>
--- a/xlsx/crawling_data.xlsx
+++ b/xlsx/crawling_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -424,16 +424,13 @@
         <v/>
       </c>
       <c r="B2" t="str">
-        <v>공과대학</v>
+        <v>건축학부</v>
       </c>
       <c r="C2" t="str">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D2" t="str">
-        <v>19</v>
-      </c>
-      <c r="E2" t="str">
-        <v>4.75 : 1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -441,16 +438,16 @@
         <v/>
       </c>
       <c r="B3" t="str">
-        <v>신소재ㆍ화공시스템공학부</v>
+        <v>건축공학부</v>
       </c>
       <c r="C3" t="str">
         <v/>
       </c>
       <c r="D3" t="str">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E3" t="str">
-        <v>5.50 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -458,16 +455,16 @@
         <v/>
       </c>
       <c r="B4" t="str">
-        <v>컴퓨터공학과</v>
+        <v>건설환경공학과</v>
       </c>
       <c r="C4" t="str">
         <v/>
       </c>
       <c r="D4" t="str">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E4" t="str">
-        <v>5.67 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -475,16 +472,16 @@
         <v/>
       </c>
       <c r="B5" t="str">
-        <v>산업ㆍ데이터공학과</v>
+        <v>도시공학과</v>
       </c>
       <c r="C5" t="str">
         <v/>
       </c>
       <c r="D5" t="str">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E5" t="str">
-        <v>6.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -492,16 +489,16 @@
         <v/>
       </c>
       <c r="B6" t="str">
-        <v>기계ㆍ시스템디자인공학과</v>
+        <v>자원환경공학과</v>
       </c>
       <c r="C6" t="str">
         <v/>
       </c>
       <c r="D6" t="str">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E6" t="str">
-        <v>4.67 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -509,16 +506,16 @@
         <v/>
       </c>
       <c r="B7" t="str">
-        <v>건설환경공학과</v>
+        <v>융합전자공학부</v>
       </c>
       <c r="C7" t="str">
         <v/>
       </c>
       <c r="D7" t="str">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="E7" t="str">
-        <v>5.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="8">
@@ -526,16 +523,16 @@
         <v/>
       </c>
       <c r="B8" t="str">
-        <v>건축학부 건축학전공(5년제)</v>
+        <v>컴퓨터소프트웨어학부</v>
       </c>
       <c r="C8" t="str">
         <v/>
       </c>
       <c r="D8" t="str">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="E8" t="str">
-        <v>7.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="9">
@@ -543,7 +540,7 @@
         <v/>
       </c>
       <c r="B9" t="str">
-        <v>건축학부 실내건축학전공</v>
+        <v>전기공학전공</v>
       </c>
       <c r="C9" t="str">
         <v/>
@@ -552,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="str">
-        <v>6.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="10">
@@ -560,16 +557,16 @@
         <v/>
       </c>
       <c r="B10" t="str">
-        <v>도시공학과</v>
+        <v>바이오메디컬공학전공</v>
       </c>
       <c r="C10" t="str">
         <v/>
       </c>
       <c r="D10" t="str">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E10" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="11">
@@ -577,16 +574,16 @@
         <v/>
       </c>
       <c r="B11" t="str">
-        <v>수학교육과</v>
+        <v>신소재공학부</v>
       </c>
       <c r="C11" t="str">
         <v/>
       </c>
       <c r="D11" t="str">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E11" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="12">
@@ -594,16 +591,16 @@
         <v/>
       </c>
       <c r="B12" t="str">
-        <v>국어교육과</v>
+        <v>화학공학과</v>
       </c>
       <c r="C12" t="str">
         <v/>
       </c>
       <c r="D12" t="str">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E12" t="str">
-        <v>6.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="13">
@@ -611,16 +608,16 @@
         <v/>
       </c>
       <c r="B13" t="str">
-        <v>영어교육과</v>
+        <v>생명공학과</v>
       </c>
       <c r="C13" t="str">
         <v/>
       </c>
       <c r="D13" t="str">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E13" t="str">
-        <v>6.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="14">
@@ -628,16 +625,16 @@
         <v/>
       </c>
       <c r="B14" t="str">
-        <v>역사교육과</v>
+        <v>유기나노공학과</v>
       </c>
       <c r="C14" t="str">
         <v/>
       </c>
       <c r="D14" t="str">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E14" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="15">
@@ -645,16 +642,16 @@
         <v/>
       </c>
       <c r="B15" t="str">
-        <v>교육학과</v>
+        <v>에너지공학과</v>
       </c>
       <c r="C15" t="str">
         <v/>
       </c>
       <c r="D15" t="str">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" t="str">
-        <v>6.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="16">
@@ -662,16 +659,16 @@
         <v/>
       </c>
       <c r="B16" t="str">
-        <v>경영학부</v>
+        <v>기계공학부</v>
       </c>
       <c r="C16" t="str">
         <v/>
       </c>
       <c r="D16" t="str">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="E16" t="str">
-        <v>7.71 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="17">
@@ -679,16 +676,16 @@
         <v/>
       </c>
       <c r="B17" t="str">
-        <v>영어영문학과</v>
+        <v>원자력공학과</v>
       </c>
       <c r="C17" t="str">
         <v/>
       </c>
       <c r="D17" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" t="str">
-        <v>5.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="18">
@@ -696,16 +693,16 @@
         <v/>
       </c>
       <c r="B18" t="str">
-        <v>독어독문학과</v>
+        <v>산업공학과</v>
       </c>
       <c r="C18" t="str">
         <v/>
       </c>
       <c r="D18" t="str">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E18" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="19">
@@ -713,16 +710,16 @@
         <v/>
       </c>
       <c r="B19" t="str">
-        <v>불어불문학과</v>
+        <v>미래자동차공학과</v>
       </c>
       <c r="C19" t="str">
         <v/>
       </c>
       <c r="D19" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E19" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="20">
@@ -730,16 +727,16 @@
         <v/>
       </c>
       <c r="B20" t="str">
-        <v>국어국문학과</v>
+        <v>데이터사이언스학부</v>
       </c>
       <c r="C20" t="str">
         <v/>
       </c>
       <c r="D20" t="str">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E20" t="str">
-        <v>3.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="21">
@@ -747,16 +744,16 @@
         <v/>
       </c>
       <c r="B21" t="str">
-        <v>법학부</v>
+        <v>수학과</v>
       </c>
       <c r="C21" t="str">
         <v/>
       </c>
       <c r="D21" t="str">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E21" t="str">
-        <v>6.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="22">
@@ -764,16 +761,16 @@
         <v/>
       </c>
       <c r="B22" t="str">
-        <v>경제학부</v>
+        <v>물리학과</v>
       </c>
       <c r="C22" t="str">
         <v/>
       </c>
       <c r="D22" t="str">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E22" t="str">
-        <v>7.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="23">
@@ -781,16 +778,16 @@
         <v/>
       </c>
       <c r="B23" t="str">
-        <v>예술학과</v>
+        <v>화학과</v>
       </c>
       <c r="C23" t="str">
         <v/>
       </c>
       <c r="D23" t="str">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E23" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="24">
@@ -798,16 +795,16 @@
         <v/>
       </c>
       <c r="B24" t="str">
-        <v>동양화과</v>
+        <v>생명과학과</v>
       </c>
       <c r="C24" t="str">
         <v/>
       </c>
       <c r="D24" t="str">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E24" t="str">
-        <v>1.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="25">
@@ -815,16 +812,16 @@
         <v/>
       </c>
       <c r="B25" t="str">
-        <v>회화과</v>
+        <v>의류학과</v>
       </c>
       <c r="C25" t="str">
         <v/>
       </c>
       <c r="D25" t="str">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E25" t="str">
-        <v>3.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="26">
@@ -832,16 +829,16 @@
         <v/>
       </c>
       <c r="B26" t="str">
-        <v>판화과</v>
+        <v>식품영양학과</v>
       </c>
       <c r="C26" t="str">
         <v/>
       </c>
       <c r="D26" t="str">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E26" t="str">
-        <v>3.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="27">
@@ -849,16 +846,16 @@
         <v/>
       </c>
       <c r="B27" t="str">
-        <v>조소과</v>
+        <v>실내건축디자인학과</v>
       </c>
       <c r="C27" t="str">
         <v/>
       </c>
       <c r="D27" t="str">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E27" t="str">
-        <v>2.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="28">
@@ -866,16 +863,16 @@
         <v/>
       </c>
       <c r="B28" t="str">
-        <v>디자인학부</v>
+        <v>간호학과</v>
       </c>
       <c r="C28" t="str">
         <v/>
       </c>
       <c r="D28" t="str">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E28" t="str">
-        <v>6.67 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="29">
@@ -883,16 +880,13 @@
         <v/>
       </c>
       <c r="B29" t="str">
-        <v>금속조형디자인과</v>
+        <v>정보시스템학과</v>
       </c>
       <c r="C29" t="str">
-        <v/>
+        <v>24</v>
       </c>
       <c r="D29" t="str">
-        <v>5</v>
-      </c>
-      <c r="E29" t="str">
-        <v>5.00 : 1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30">
@@ -900,16 +894,16 @@
         <v/>
       </c>
       <c r="B30" t="str">
-        <v>도예ㆍ유리과</v>
+        <v>국어국문학과</v>
       </c>
       <c r="C30" t="str">
         <v/>
       </c>
       <c r="D30" t="str">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E30" t="str">
-        <v>4.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="31">
@@ -917,16 +911,16 @@
         <v/>
       </c>
       <c r="B31" t="str">
-        <v>목조형가구학과</v>
+        <v>중어중문학과</v>
       </c>
       <c r="C31" t="str">
         <v/>
       </c>
       <c r="D31" t="str">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E31" t="str">
-        <v>2.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="32">
@@ -934,16 +928,16 @@
         <v/>
       </c>
       <c r="B32" t="str">
-        <v>섬유미술ㆍ패션디자인과</v>
+        <v>영어영문학과</v>
       </c>
       <c r="C32" t="str">
         <v/>
       </c>
       <c r="D32" t="str">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" t="str">
-        <v>7.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="33">
@@ -951,16 +945,16 @@
         <v/>
       </c>
       <c r="B33" t="str">
-        <v>과학기술대학</v>
+        <v>독어독문학과</v>
       </c>
       <c r="C33" t="str">
-        <v>8</v>
+        <v/>
       </c>
       <c r="D33" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E33" t="str">
-        <v>0.25 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="34">
@@ -968,13 +962,13 @@
         <v/>
       </c>
       <c r="B34" t="str">
-        <v>소프트웨어융합학과</v>
+        <v>사학과</v>
       </c>
       <c r="C34" t="str">
         <v/>
       </c>
       <c r="D34" t="str">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E34" t="str">
         <v/>
@@ -985,13 +979,13 @@
         <v/>
       </c>
       <c r="B35" t="str">
-        <v>나노신소재학과</v>
+        <v>철학과</v>
       </c>
       <c r="C35" t="str">
         <v/>
       </c>
       <c r="D35" t="str">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E35" t="str">
         <v/>
@@ -1002,13 +996,13 @@
         <v/>
       </c>
       <c r="B36" t="str">
-        <v>건축공학부</v>
+        <v>정치외교학과</v>
       </c>
       <c r="C36" t="str">
         <v/>
       </c>
       <c r="D36" t="str">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E36" t="str">
         <v/>
@@ -1019,13 +1013,13 @@
         <v/>
       </c>
       <c r="B37" t="str">
-        <v>기계정보공학과</v>
+        <v>사회학과</v>
       </c>
       <c r="C37" t="str">
         <v/>
       </c>
       <c r="D37" t="str">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E37" t="str">
         <v/>
@@ -1036,13 +1030,13 @@
         <v/>
       </c>
       <c r="B38" t="str">
-        <v>조선해양공학과</v>
+        <v>미디어커뮤니케이션학과</v>
       </c>
       <c r="C38" t="str">
         <v/>
       </c>
       <c r="D38" t="str">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="E38" t="str">
         <v/>
@@ -1053,13 +1047,13 @@
         <v/>
       </c>
       <c r="B39" t="str">
-        <v>바이오화학공학과</v>
+        <v>관광학부</v>
       </c>
       <c r="C39" t="str">
         <v/>
       </c>
       <c r="D39" t="str">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E39" t="str">
         <v/>
@@ -1070,16 +1064,16 @@
         <v/>
       </c>
       <c r="B40" t="str">
-        <v>게임학부 게임소프트웨어전공(공학계)</v>
+        <v>정책학과</v>
       </c>
       <c r="C40" t="str">
         <v/>
       </c>
       <c r="D40" t="str">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E40" t="str">
-        <v>0.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="41">
@@ -1087,16 +1081,16 @@
         <v/>
       </c>
       <c r="B41" t="str">
-        <v>상경학부</v>
+        <v>행정학과</v>
       </c>
       <c r="C41" t="str">
         <v/>
       </c>
       <c r="D41" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E41" t="str">
-        <v>0.00 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="42">
@@ -1104,16 +1098,16 @@
         <v/>
       </c>
       <c r="B42" t="str">
-        <v>광고홍보학부</v>
+        <v>경제금융학부</v>
       </c>
       <c r="C42" t="str">
         <v/>
       </c>
       <c r="D42" t="str">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="E42" t="str">
-        <v>0.67 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="43">
@@ -1121,16 +1115,16 @@
         <v/>
       </c>
       <c r="B43" t="str">
-        <v>디자인컨버전스학부</v>
+        <v>경영학부</v>
       </c>
       <c r="C43" t="str">
         <v/>
       </c>
       <c r="D43" t="str">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="E43" t="str">
-        <v>2.50 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="44">
@@ -1138,16 +1132,16 @@
         <v/>
       </c>
       <c r="B44" t="str">
-        <v>영상애니메이션학부</v>
+        <v>파이낸스경영학과</v>
       </c>
       <c r="C44" t="str">
         <v/>
       </c>
       <c r="D44" t="str">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E44" t="str">
-        <v>2.50 : 1</v>
+        <v/>
       </c>
     </row>
     <row r="45">
@@ -1155,21 +1149,52 @@
         <v/>
       </c>
       <c r="B45" t="str">
-        <v>게임학부 게임그래픽디자인전공(미술계)</v>
+        <v>스포츠매니지먼트전공</v>
       </c>
       <c r="C45" t="str">
         <v/>
       </c>
       <c r="D45" t="str">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E45" t="str">
-        <v>2.00 : 1</v>
+        <v/>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v/>
+      </c>
+      <c r="B46" t="str">
+        <v>연극영화학과(영화전공)</v>
+      </c>
+      <c r="C46" t="str">
+        <v/>
+      </c>
+      <c r="D46" t="str">
+        <v>9</v>
+      </c>
+      <c r="E46" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v/>
+      </c>
+      <c r="B47" t="str">
+        <v>국제학전공</v>
+      </c>
+      <c r="C47" t="str">
+        <v>3</v>
+      </c>
+      <c r="D47" t="str">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E45"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>